<commit_message>
edited leg xlsx and added some cleaning boilerplate from a tutorial my colleague wrote - it is not updated yet
</commit_message>
<xml_diff>
--- a/template legislation.xlsx
+++ b/template legislation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DAE550-3FD3-494E-92F8-C93DC4C14E43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736D9821-9E44-4B79-9E86-E3E144F9A094}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,52 +393,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" customWidth="1"/>
-    <col min="5" max="5" width="30.54296875" customWidth="1"/>
-    <col min="6" max="6" width="88.08984375" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="4" max="4" width="30.54296875" customWidth="1"/>
+    <col min="5" max="5" width="88.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>